<commit_message>
V3.0 + new BOM
</commit_message>
<xml_diff>
--- a/System_development/Pelican/structural_model/v0.2.4/BOM/BOM.xlsx
+++ b/System_development/Pelican/structural_model/v0.2.4/BOM/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SWIFT-UAV\System_development\Pelican\structural_model\v0.2.4\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5C2F4E-3D0D-4A8E-90BE-818BB41E7D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84CC5F2-C322-4333-9A9E-0DB3D70255F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{592DD08D-685A-4368-B045-771DD756553C}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>https://mad-motor.com/products/mad-ampx-esc-120a-5-14s?VariantsId=10934</t>
   </si>
   <si>
-    <t>https://mad-motor.com/products/mad-components-brushless-motor-x7215?VariantsId=10591</t>
-  </si>
-  <si>
     <t>3D Printed</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>M6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -534,17 +534,17 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +558,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -566,13 +566,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -580,13 +580,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -594,13 +594,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -608,13 +608,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -622,29 +622,29 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <f>3+3+4</f>
@@ -655,49 +655,49 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -705,27 +705,27 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -733,13 +733,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -747,13 +747,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -767,37 +767,37 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -807,7 +807,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -815,7 +815,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -823,7 +823,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -831,7 +831,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -839,7 +839,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -847,7 +847,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -855,7 +855,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -863,7 +863,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -871,7 +871,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -879,7 +879,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -887,7 +887,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -895,7 +895,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -903,7 +903,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -911,7 +911,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -919,7 +919,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -927,7 +927,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -935,21 +935,21 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -957,7 +957,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" xr:uid="{5A87A4CA-4739-4D3C-AC79-A6DBEDA8C270}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{05A004DB-B4EC-4253-8E67-A2DF5F46427B}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://mad-motor.com/products/mad-components-brushless-motor-x7215?VariantsId=10591" xr:uid="{05A004DB-B4EC-4253-8E67-A2DF5F46427B}"/>
     <hyperlink ref="C12" r:id="rId3" xr:uid="{481D7C56-D89E-49EC-8E7C-B3B970929588}"/>
     <hyperlink ref="C18" r:id="rId4" xr:uid="{3EE96FE7-F3E1-4B99-827B-A3E813BCF243}"/>
     <hyperlink ref="C17" r:id="rId5" xr:uid="{140CD40A-BBC7-4229-A5D2-16F062B375BE}"/>

</xml_diff>